<commit_message>
Minor correction of a name
</commit_message>
<xml_diff>
--- a/hardware/manufacturing/Stackup/SwiftMoteECp_Stackup_v1.1.xlsx
+++ b/hardware/manufacturing/Stackup/SwiftMoteECp_Stackup_v1.1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\one\co_kicad6\ratkit\ratkit_proto\rkp_hw\ratkit_design\manufacturing\Stackup\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cmcgit\SwiftMoteEC_HW_forkPub\hardware\manufacturing\Stackup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA3B05EF-C318-4A2E-986F-7F04798E989F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1704D51-6605-417C-8091-6043A5A92190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24330" yWindow="885" windowWidth="21600" windowHeight="13515" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Stackup_1.1" sheetId="2" r:id="rId1"/>
@@ -79,9 +79,6 @@
     <t>RatKit_proto_2022A</t>
   </si>
   <si>
-    <t>RatKit_proto_2022A - Stackup</t>
-  </si>
-  <si>
     <t>PWRp</t>
   </si>
   <si>
@@ -158,6 +155,9 @@
   </si>
   <si>
     <t>FAB=0.063 MILS +/-8MILS</t>
+  </si>
+  <si>
+    <t>SwiftMote_proto_2022A - Stackup</t>
   </si>
 </sst>
 </file>
@@ -234,26 +234,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -539,432 +529,357 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9695371E-8DD9-4302-8155-173F095D2392}">
-  <dimension ref="A2:H34"/>
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A2:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17" style="10" customWidth="1"/>
-    <col min="3" max="3" width="11.5703125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="16.5703125" style="10" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17" customWidth="1"/>
+    <col min="3" max="3" width="11.5703125" customWidth="1"/>
+    <col min="4" max="5" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3"/>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="1"/>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="E3" s="9"/>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="18" t="s">
+      <c r="E3" s="4"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="18"/>
-      <c r="D4" s="19">
+      <c r="C4" s="8"/>
+      <c r="D4" s="9">
         <f>E30</f>
         <v>63.800000000000011</v>
       </c>
-      <c r="E4" s="9" t="s">
+      <c r="E4" s="4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="1"/>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="9" t="s">
+      <c r="E5" s="4" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="18" t="s">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="18"/>
-      <c r="D6" s="19" t="s">
+      <c r="C6" s="8"/>
+      <c r="D6" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="E6" s="9"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="18" t="s">
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="19">
+      <c r="C7" s="8"/>
+      <c r="D7" s="9">
         <v>4.04</v>
       </c>
-      <c r="E7" s="9"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="7"/>
-      <c r="B8" s="11"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="8" t="s">
-        <v>38</v>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E8" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="8"/>
-      <c r="B9" s="12" t="s">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E9" s="12" t="s">
+      <c r="E9" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" s="1"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E10" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="7">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E13" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="2"/>
+      <c r="D18" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="E18" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="G18" s="1"/>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E19" s="7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C20" s="2"/>
+      <c r="D20" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="2">
+        <v>1.2</v>
+      </c>
+      <c r="G20" s="1"/>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="7">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E23" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E25" s="7">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="E27" s="7">
+        <v>5.4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="2">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2" t="s">
         <v>35</v>
-      </c>
-      <c r="F9" s="4"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="4"/>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="F10" s="4"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="4"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="8"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="17">
-        <v>5.4</v>
-      </c>
-      <c r="F11" s="4"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="4"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="7"/>
-      <c r="B12" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E12" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="F12" s="4"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="4"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="8"/>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="17">
-        <v>7</v>
-      </c>
-      <c r="F13" s="4"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="4"/>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="7"/>
-      <c r="B14" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="E14" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="4"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="8"/>
-      <c r="B15" s="13"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E15" s="17">
-        <v>7</v>
-      </c>
-      <c r="F15" s="4"/>
-      <c r="G15" s="7"/>
-      <c r="H15" s="4"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="7"/>
-      <c r="B16" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E16" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="F16" s="4"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="4"/>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="8"/>
-      <c r="B17" s="13"/>
-      <c r="C17" s="13"/>
-      <c r="D17" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="17">
-        <v>4</v>
-      </c>
-      <c r="F17" s="4"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="4"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="7"/>
-      <c r="B18" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="E18" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="F18" s="4"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="4"/>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="8"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="14"/>
-      <c r="D19" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E19" s="17">
-        <v>5</v>
-      </c>
-      <c r="F19" s="4"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="4"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="7"/>
-      <c r="B20" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="C20" s="13"/>
-      <c r="D20" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="F20" s="4"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="4"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="7"/>
-      <c r="B21" s="13"/>
-      <c r="C21" s="13"/>
-      <c r="D21" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="17">
-        <v>4</v>
-      </c>
-      <c r="F21" s="4"/>
-      <c r="G21" s="7"/>
-      <c r="H21" s="4"/>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="7"/>
-      <c r="B22" s="13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="13"/>
-      <c r="D22" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E22" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="F22" s="4"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="4"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="7"/>
-      <c r="B23" s="13"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="E23" s="17">
-        <v>7</v>
-      </c>
-      <c r="F23" s="4"/>
-      <c r="G23" s="7"/>
-      <c r="H23" s="4"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="7"/>
-      <c r="B24" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="C24" s="13"/>
-      <c r="D24" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="E24" s="6">
-        <v>1.2</v>
-      </c>
-      <c r="F24" s="4"/>
-      <c r="G24" s="7"/>
-      <c r="H24" s="4"/>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="13"/>
-      <c r="C25" s="13"/>
-      <c r="D25" s="16" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="17">
-        <v>7</v>
-      </c>
-      <c r="F25" s="4"/>
-      <c r="G25" s="7"/>
-      <c r="H25" s="4"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C26" s="14"/>
-      <c r="D26" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
-      <c r="H26" s="4"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="14"/>
-      <c r="C27" s="14"/>
-      <c r="D27" s="16" t="s">
-        <v>33</v>
-      </c>
-      <c r="E27" s="17">
-        <v>5.4</v>
-      </c>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="14"/>
-      <c r="D28" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="E28" s="2">
-        <v>1.2</v>
-      </c>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
-      <c r="H28" s="4"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="14"/>
-      <c r="C29" s="14"/>
-      <c r="D29" s="14"/>
-      <c r="E29" s="2"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="14"/>
-      <c r="C30" s="14"/>
-      <c r="D30" s="14" t="s">
-        <v>36</v>
       </c>
       <c r="E30" s="2">
         <f>SUM(E10:E28)</f>
         <v>63.800000000000011</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="G30" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H30" s="4"/>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="D32" s="11" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="G30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D32" t="s">
+        <v>36</v>
       </c>
       <c r="E32">
         <f>E30/10</f>
@@ -973,11 +888,11 @@
     </row>
     <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+  <pageSetup scale="79" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Minor correction of a name, take 2
</commit_message>
<xml_diff>
--- a/hardware/manufacturing/Stackup/SwiftMoteECp_Stackup_v1.1.xlsx
+++ b/hardware/manufacturing/Stackup/SwiftMoteECp_Stackup_v1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cmcgit\SwiftMoteEC_HW_forkPub\hardware\manufacturing\Stackup\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1704D51-6605-417C-8091-6043A5A92190}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CBCF386E-E7B0-47DB-84AC-E1B3987406CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -157,7 +157,7 @@
     <t>FAB=0.063 MILS +/-8MILS</t>
   </si>
   <si>
-    <t>SwiftMote_proto_2022A - Stackup</t>
+    <t>SwiftMoteEC_proto_2022A - Stackup</t>
   </si>
 </sst>
 </file>
@@ -535,7 +535,7 @@
   <dimension ref="A2:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>